<commit_message>
find all map, write to excel to one sheet
</commit_message>
<xml_diff>
--- a/Шторм.xlsx
+++ b/Шторм.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,6 +437,21 @@
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -449,6 +464,31 @@
           <t>Please enter the complete name</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>已存在</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Введите полное имя</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>الرجاء إدخال الاسم الكامل</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Veuillez entrer le nom complet</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Por favor, ingrese el nombre completo</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -461,6 +501,31 @@
           <t>This operation will add a hidden mapping relationship between the frequency point and rate of this detection result. Due to the deviation jitter of the mapped rate within ±500, it may affect other detection results within this range. Do you want to continue?</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>请输入完整的名称</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Это добавит скрытое отображение отношения частоты и скорости результата обнаружения. Это может повлиять на другие результаты обнаружения в этом диапазоне. Хотите продолжить?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>سيؤدي هذا الإجراء إلى إضافة علاقة تعيين مخفية بين نقطة التردد والمعدل لنتيجة الكشف هذه. نظرًا لتذبذب الانحراف للمعدل المعين ضمن ±500 ، قد يؤثر هذا على نتائج الكشف الأخرى ضمن هذا النطاق. هل ترغب في المتابعة؟</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cette opération ajoutera une relation de mappage masquée entre le point de fréquence et le taux de ce résultat de détection. En raison des fluctuations de déviation de ±500 du taux mappé, cela peut affecter d'autres résultats de détection dans cette plage. Voulez-vous continuer ?</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Esta operación agregará una relación de mapeo oculta entre el punto de frecuencia y la tasa de este resultado de detección. Debido a la fluctuación de desviación de ±500 en la tasa mapeada, esto puede afectar a otros resultados de detección dentro de este rango. ¿Desea continuar?</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -473,6 +538,31 @@
           <t>Hide</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>该操作将添加此探测结果的 频点与rate的 隐藏映射关系,由于映射的rate有上下500偏差抖动, 可能会影响其他除以此范围的探测结果 是否继续?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Скрыть</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>إخفاء</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Masquer</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ocultar</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -485,6 +575,31 @@
           <t>X1C</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>屏蔽</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X1C</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>X1C</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>X1C</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>X1C</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -497,6 +612,31 @@
           <t>Amplifier</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>侦测定位</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Усилитель</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>المضخم</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>amplificateur</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>amplificador</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -509,6 +649,31 @@
           <t>Double click to end measurement</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>功放</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Дважды щелкните, чтобы завершить измерение</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>انقر نقرًا مزدوجًا لإنهاء القياس</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Double-cliquez pour terminer la mesure</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Haga doble clic para finalizar la medición</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -521,6 +686,31 @@
           <t>Defense settings</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>反制控制</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Настройки защиты</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>إعدادات الضربة</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>paramètres de grève</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ajustes de huelga</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -533,6 +723,31 @@
           <t>manual strike</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>双击结束测量</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Ручное подавление</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ضربة يدوية</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Frappe manuelle</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Golpe manual</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -545,6 +760,31 @@
           <t>Defense settings</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>打击设置</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Подавить</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>يضرب</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Frappe</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Golpe</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -557,6 +797,31 @@
           <t>Reload map</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>手动打击</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Перезагрузить карту</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>إعادة تحميل الخريطة</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Recharger la carte</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Reiniciar mapa</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -569,6 +834,31 @@
           <t>List</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>打击</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Список</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>القائمة</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>liste</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Lista</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -581,6 +871,31 @@
           <t>Portable Drone detection and positioning equipment</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>地图复位</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Обнаружение и позиционирование дронов</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>معدات الكشف عن الطائرات بدون طيار وتحديد المواقع</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Equipement portable de détection et positionnement de Drone</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Equipo de ubicación y detección de drones portátil</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -593,6 +908,31 @@
           <t>clear</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>列表</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Пустой</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>فارغ</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Vider</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Limpiar</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -605,6 +945,31 @@
           <t>En</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>手提式无人机侦测定位设备</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Английский</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>إنجليزي</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Anglais</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Inglés</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -617,6 +982,31 @@
           <t>Copy</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>清空</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Копировать</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ينسخ</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Copier</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Copiar</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -629,6 +1019,31 @@
           <t>Copy coordinates</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>英文</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Скопировать координаты</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>نسخ الإحداثيات</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Copier des coordonnées</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Copiar coordenadas</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -641,6 +1056,31 @@
           <t>Click coordinates</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>复制</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Нажмите на координаты</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>انقر فوق الإحداثيات</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Cliquez sur des coordonnées</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Haga clic en las coordenadas</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -653,6 +1093,31 @@
           <t>Search coordinates</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>复制坐标</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Координаты поиска</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>إحداثيات البحث</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Rechercher des coordonnées</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Buscar coordenadas</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -665,6 +1130,31 @@
           <t>Coordinate picker</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>点击坐标</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Средство выбора координат</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>تنسيق المنتقي</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Sélecteur de coordonnées</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Selector de coordenadas</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -677,6 +1167,31 @@
           <t>Add to trust</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>搜索坐标</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Добавить в список доверенных</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>أضف الثقة</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ajouter à la liste de confiance</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Agregar confianza</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -689,6 +1204,31 @@
           <t>Trust</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>坐标拾取器</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Доверять</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>يثق</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Confiance</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Confianza</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -701,6 +1241,31 @@
           <t>Download map</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>添加信任</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Скачать карту</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>تحميل الخريطة</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Télécharger la carte</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Descargar mapa</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -713,6 +1278,31 @@
           <t>The map file is large, under evaluation...</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>信任</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Файл карты большой, оцениавется...</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ملف الخريطة كبير قيد التقييم ...</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Le fichier de la carte est volumineux, en cours d'évaluation...</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>El archivo de mapa es grande, evaluando...</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -725,6 +1315,31 @@
           <t>close</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>下载地图</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Закрыть</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>إنهاء</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>fermer</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Cerrar</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -737,6 +1352,31 @@
           <t>register</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>地图文件较大, 评估中...</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Регистрация</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>يسجل</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>enregistrer</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Registrarse</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -749,6 +1389,31 @@
           <t>login</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>关闭</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Авторизоваться</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>تسجيل الدخول</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>connexion</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Iniciar sesión</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -761,6 +1426,31 @@
           <t>username</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>注册</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Имя пользователя</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>اسم المستخدم</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>nom d’utilisateur</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nombre de usuario</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -773,6 +1463,31 @@
           <t>password</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>登录</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Пароль</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>كلمة المرور</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>mot de passe</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Contraseña</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -785,6 +1500,31 @@
           <t>Add</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>用户名</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Добавить</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>اضف إليه</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>ajouter</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Agregar</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -797,6 +1537,31 @@
           <t>Drone name</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>密码</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Имя дрона</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>اسم الطائرة بدون طيار</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>nom de Drone</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Nombre del dron</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -809,6 +1574,31 @@
           <t>delete</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>添加</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Удалить</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>يمسح</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>supprimer</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Eliminar</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -821,6 +1611,31 @@
           <t>Operate</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>无人机名</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Действовать</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>العمل</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Opérer</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Operar</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -833,6 +1648,31 @@
           <t>Name</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>删除</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Название</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>اسم</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>nom</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -845,6 +1685,31 @@
           <t>Drone id</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>操作</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Идентификатор дрона</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>معرف الطائرة بدون طيار</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Identifiant du Drone</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>ID del dron</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -857,6 +1722,31 @@
           <t>White list</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>名称</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Белый список</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>القائمة البيضاء</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>liste blanche</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Lista blanca</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -869,6 +1759,31 @@
           <t>Set</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>无人机ID</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Настройки системы</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>اعدادات النظام</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Configuration du système</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Configuración del sistema</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -881,6 +1796,31 @@
           <t>Settings</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>白名单列表</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Настроить</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>يثبت</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>paramètres</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Configuración</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -893,6 +1833,31 @@
           <t>Flight path playback</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>系统设置</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Воспроизведение трека</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>تشغيل المسار</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Lecture de trajctoires de vol</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Reproducción de la trayectoria</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -905,6 +1870,31 @@
           <t>Record list</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>设置</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Журнал</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>قائمة التسجيلات</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>liste des enregistrements</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Lista de registros</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -917,6 +1907,31 @@
           <t>Data analytics</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>轨迹回放</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Анализ данных</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>تحليل البيانات</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>analyse des données</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Análisis de datos</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -929,6 +1944,31 @@
           <t>Measure distance</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>记录列表</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Линейка</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>أداة قياس المسافة</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Outil de mesure des distances</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Herramienta de medición de distancias</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -941,6 +1981,31 @@
           <t>Extract coordinates</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>数据分析</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Извлечение координат</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>تنسيق الاستخراج</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Extraire des coordonnées</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Extracción de coordenadas</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -953,6 +2018,31 @@
           <t>Device restart</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>测距工具</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Перезагрузите устройство</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>أعد تشغيل الجهاز</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Redémarrer l'appareil</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Reiniciar dispositivo</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -965,6 +2055,31 @@
           <t>Clear flight</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>坐标提取</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Очистить путь</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>مسار واضح</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Effacer la trajectoire de vol</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Borrar trayectoria</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -977,6 +2092,31 @@
           <t>AMap</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>重启设备</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Карта Гаоде</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>خريطة Gaode</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>AMap</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Mapa AMap</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -989,6 +2129,31 @@
           <t>BaiduMap</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>清除轨迹</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Карта Байду</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>خريطة بايدو</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>BaiduMap</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Mapa Baidu</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -1001,6 +2166,31 @@
           <t>BingMap</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>高德地图</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Карты Бинга</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>خرائط بنج</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>BingMap</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Mapa Bing</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -1013,6 +2203,31 @@
           <t>AMapStreet</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>百度地图</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Гаоде-стрит</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>شارع Gaode</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>AMapStreet</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Calles AMap</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1025,6 +2240,31 @@
           <t>GoogleMap</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>必应地图</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Google Map</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>خرائط جوجل</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>GoogleMap</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Mapa de Google</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1037,6 +2277,31 @@
           <t>AMapHybird</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>高德街道</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Спутник Гаоде</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>القمر الصناعي Gaode</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>AMapHybird</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Satélite AMap</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1049,6 +2314,31 @@
           <t>GCJ02Street</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>谷歌地图</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>улица GCJ02</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>شارع GCJ02</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>GCJ-02Street</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Calles GCJ02</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1061,6 +2351,31 @@
           <t>TencentMap</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>高德卫星</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Карта Тенсент</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>خريطة تينسنت</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>TencentMap</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Mapa Tx</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1073,6 +2388,31 @@
           <t>Drone list</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>GCJ02街道</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Дроны</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>قائمة الطائرات بدون طيار</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>liste de Drones</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Lista de drones</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -1085,6 +2425,31 @@
           <t>color</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>腾讯地图</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Цвет</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>لون</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>couleur</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -1097,6 +2462,31 @@
           <t>Model</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>无人机列表</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Модель</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>نموذج</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>modèle</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -1109,6 +2499,31 @@
           <t>Azimuth distance</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>颜色</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Расстояние по азимуту</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>مسافة السمت</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>distance azimutale</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Distancia de azimuth</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1121,6 +2536,31 @@
           <t>Device ID</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>型号</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>ID устройства</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>معرف الجهاز</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Identifiant d’appareil</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>ID del dispositivo</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1133,6 +2573,31 @@
           <t>Update time</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>方位距离</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Время обновления</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>تحديث الوقت</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Heure de mise à jour</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Tiempo de actualización</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -1145,6 +2610,31 @@
           <t>Frequency</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>设备ID</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>частота</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>تكرار</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>fréquence</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Frecuencia</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -1157,6 +2647,31 @@
           <t>Bandwidth</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>更新时间</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Пропускная способность</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>عرض النطاق</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>bande passante</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Ancho de banda</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -1169,6 +2684,31 @@
           <t>decode</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>频率</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Расшифровать</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>يحسن</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>décoder</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Mejora</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -1181,6 +2721,31 @@
           <t>Detect</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>带宽</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Обнаружение</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>كشف</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>détecter</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Detección</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -1193,6 +2758,31 @@
           <t>online</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>增强</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Онлайн</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>متصل</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>en ligne</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>En línea</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -1205,6 +2795,31 @@
           <t>offline</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>探测</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Офлайн</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>غير متصل بالانترنت</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>hors ligne</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Fuera de línea</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -1217,6 +2832,31 @@
           <t>Detect List</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>在线</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Дроны</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>قائمة التحقيق</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Liste de détection</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Lista de detección</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -1229,6 +2869,31 @@
           <t>Locate/Detect</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>离线</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Найти/обнаружить</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>حدد / كشف</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>localiser/détecter</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Ubicar/Detectar</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -1241,6 +2906,31 @@
           <t>Detection Result</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>探测列表</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Результаты</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>قائمة النتائج</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>résultat de détection</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Lista de resultados</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -1253,6 +2943,31 @@
           <t>Pilot</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>定位/探测</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Значок пилота</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>رمز الطيار</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Icône de pilote</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Icono del piloto</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -1265,6 +2980,31 @@
           <t>Location</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>结果列表</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Переключатель дисплея</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>تبديل العرض</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>localisation</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Interruptor de visualización</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -1277,6 +3017,31 @@
           <t>download</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>飞手图标</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Скачать</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>تحميل</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>télécharger</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Descargar</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -1289,6 +3054,31 @@
           <t>update scenario error</t>
         </is>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>显示开关</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Не удалось обновить сценарий</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>فشل تحديث الخطة</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>erreur de mise à jour de scénario</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Error al actualizar el plan</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -1301,6 +3091,31 @@
           <t>get scenario error</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>下载</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Не удалось получить сценарий</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>فشل في الحصول على الخطة</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>erreur d’obtention de scénario</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Error al obtener el plan</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
@@ -1311,6 +3126,45 @@
       <c r="B74" t="inlineStr">
         <is>
           <t>edit</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>更新预案失败</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Редактировать</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>يحرر</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>modifier</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Editar</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>获取预案失败</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>编辑</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding more parts, error with : in values
</commit_message>
<xml_diff>
--- a/Шторм.xlsx
+++ b/Шторм.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,1241 +448,3074 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>nameCannotNull</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Please enter the complete name</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Введите полное имя</t>
+          <t>map:</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>addHideRateTips</t>
+          <t>nameCannotNull</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This operation will add a hidden mapping relationship between the frequency point and rate of this detection result. Due to the deviation jitter of the mapped rate within ±500, it may affect other detection results within this range. Do you want to continue?</t>
+          <t>Please enter the complete name</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Это добавит скрытое отображение отношения частоты и скорости результата обнаружения. Это может повлиять на другие результаты обнаружения в этом диапазоне. Хотите продолжить?</t>
+          <t>Введите полное имя</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>hide</t>
+          <t>addHideRateTips</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hide</t>
+          <t>This operation will add a hidden mapping relationship between the frequency point and rate of this detection result. Due to the deviation jitter of the mapped rate within ±500, it may affect other detection results within this range. Do you want to continue?</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Скрыть</t>
+          <t>Это добавит скрытое отображение отношения частоты и скорости результата обнаружения. Это может повлиять на другие результаты обнаружения в этом диапазоне. Хотите продолжить?</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>X1C</t>
+          <t>hide</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>X1C</t>
+          <t>Hide</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>X1C</t>
+          <t>Скрыть</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>amplifier</t>
+          <t>X1C</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Amplifier</t>
+          <t>X1C</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Усилитель</t>
+          <t>X1C</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>endMeasure</t>
+          <t>amplifier</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Double click to end measurement</t>
+          <t>Amplifier</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Дважды щелкните, чтобы завершить измерение</t>
+          <t>Усилитель</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>strikeSettings</t>
+          <t>endMeasure</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Defense settings</t>
+          <t>Double click to end measurement</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Настройки защиты</t>
+          <t>Дважды щелкните, чтобы завершить измерение</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>manualStrike</t>
+          <t>strikeSettings</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>manual strike</t>
+          <t>Defense settings</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ручное подавление</t>
+          <t>Настройки защиты</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>strike</t>
+          <t>manualStrike</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Defense settings</t>
+          <t>manual strike</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Подавить</t>
+          <t>Ручное подавление</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>mapReload</t>
+          <t>strike</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Reload map</t>
+          <t>Defense settings</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Перезагрузить карту</t>
+          <t>Подавить</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>list</t>
+          <t>mapReload</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>List</t>
+          <t>Reload map</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Список</t>
+          <t>Перезагрузить карту</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>defaultTitle</t>
+          <t>list</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Portable Drone detection and positioning equipment</t>
+          <t>List</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Обнаружение и позиционирование дронов</t>
+          <t>Список</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>clear</t>
+          <t>defaultTitle</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>clear</t>
+          <t>Portable Drone detection and positioning equipment</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Пустой</t>
+          <t>Обнаружение и позиционирование дронов</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>english</t>
+          <t>clear</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>En</t>
+          <t>clear</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Английский</t>
+          <t>Пустой</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>copy</t>
+          <t>english</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Copy</t>
+          <t>En</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Копировать</t>
+          <t>Английский</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>copyCoordinates</t>
+          <t>copy</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Copy coordinates</t>
+          <t>Copy</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Скопировать координаты</t>
+          <t>Копировать</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>clickCoordinates</t>
+          <t>copyCoordinates</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Click coordinates</t>
+          <t>Copy coordinates</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Нажмите на координаты</t>
+          <t>Скопировать координаты</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>coordinateSearch</t>
+          <t>clickCoordinates</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Search coordinates</t>
+          <t>Click coordinates</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Координаты поиска</t>
+          <t>Нажмите на координаты</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>coordinatePicker</t>
+          <t>coordinateSearch</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Coordinate picker</t>
+          <t>Search coordinates</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Средство выбора координат</t>
+          <t>Координаты поиска</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>addWhite</t>
+          <t>coordinatePicker</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Add to trust</t>
+          <t>Coordinate picker</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Добавить в список доверенных</t>
+          <t>Средство выбора координат</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>trust</t>
+          <t>addWhite</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Trust</t>
+          <t>Add to trust</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Доверять</t>
+          <t>Добавить в список доверенных</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>downloadMap</t>
+          <t>trust</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Download map</t>
+          <t>Trust</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Скачать карту</t>
+          <t>Доверять</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>preparationTips</t>
+          <t>downloadMap</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>The map file is large, under evaluation...</t>
+          <t>Download map</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Файл карты большой, оцениавется...</t>
+          <t>Скачать карту</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>close</t>
+          <t>preparationTips</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>close</t>
+          <t>The map file is large, under evaluation...</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Закрыть</t>
+          <t>Файл карты большой, оцениавется...</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>register</t>
+          <t>close</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>register</t>
+          <t>close</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Регистрация</t>
+          <t>Закрыть</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>register</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>register</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Авторизоваться</t>
+          <t>Регистрация</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>username</t>
+          <t>login</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>username</t>
+          <t>login</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Имя пользователя</t>
+          <t>Авторизоваться</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>password</t>
+          <t>username</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>password</t>
+          <t>username</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Пароль</t>
+          <t>Имя пользователя</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>add</t>
+          <t>password</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Add</t>
+          <t>password</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Добавить</t>
+          <t>Пароль</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>droneName</t>
+          <t>add</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Drone name</t>
+          <t>Add</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Имя дрона</t>
+          <t>Добавить</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>delete</t>
+          <t>droneName</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>delete</t>
+          <t>Drone name</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Удалить</t>
+          <t>Имя дрона</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>operate</t>
+          <t>delete</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Operate</t>
+          <t>delete</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Действовать</t>
+          <t>Удалить</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>operate</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Operate</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Название</t>
+          <t>Действовать</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>droneID</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Drone id</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Идентификатор дрона</t>
+          <t>Название</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>whiteList</t>
+          <t>droneID</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>White list</t>
+          <t>Drone id</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Белый список</t>
+          <t>Идентификатор дрона</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>set</t>
+          <t>whiteList</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Set</t>
+          <t>White list</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Настройки системы</t>
+          <t>Белый список</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>setTitle</t>
+          <t>set</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Settings</t>
+          <t>Set</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Настроить</t>
+          <t>Настройки системы</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>playBack</t>
+          <t>setTitle</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Flight path playback</t>
+          <t>Settings</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Воспроизведение трека</t>
+          <t>Настроить</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>recordList</t>
+          <t>playBack</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Record list</t>
+          <t>Flight path playback</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Журнал</t>
+          <t>Воспроизведение трека</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>dataAnalysis</t>
+          <t>recordList</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Data analytics</t>
+          <t>Record list</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Анализ данных</t>
+          <t>Журнал</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>distanceTool</t>
+          <t>dataAnalysis</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Measure distance</t>
+          <t>Data analytics</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Линейка</t>
+          <t>Анализ данных</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>coordinate</t>
+          <t>distanceTool</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Extract coordinates</t>
+          <t>Measure distance</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Извлечение координат</t>
+          <t>Линейка</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>deviceRestart</t>
+          <t>coordinate</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Device restart</t>
+          <t>Extract coordinates</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Перезагрузите устройство</t>
+          <t>Извлечение координат</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>clearTrack</t>
+          <t>deviceRestart</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Clear flight</t>
+          <t>Device restart</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Очистить путь</t>
+          <t>Перезагрузите устройство</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>AMap</t>
+          <t>clearTrack</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>AMap</t>
+          <t>Clear flight</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Карта Гаоде</t>
+          <t>Очистить путь</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>BaiduMap</t>
+          <t>AMap</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>BaiduMap</t>
+          <t>AMap</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Карта Байду</t>
+          <t>Карта Гаоде</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>BingMap</t>
+          <t>BaiduMap</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>BingMap</t>
+          <t>BaiduMap</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Карты Бинга</t>
+          <t>Карта Байду</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>AMapStreet</t>
+          <t>BingMap</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>AMapStreet</t>
+          <t>BingMap</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Гаоде-стрит</t>
+          <t>Карты Бинга</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>GooleMap</t>
+          <t>AMapStreet</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>GoogleMap</t>
+          <t>AMapStreet</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Google Map</t>
+          <t>Гаоде-стрит</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>AMapHybird</t>
+          <t>GooleMap</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AMapHybird</t>
+          <t>GoogleMap</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Спутник Гаоде</t>
+          <t>Google Map</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>GCJ02Street</t>
+          <t>AMapHybird</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>GCJ02Street</t>
+          <t>AMapHybird</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>улица GCJ02</t>
+          <t>Спутник Гаоде</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>TxMap</t>
+          <t>GCJ02Street</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>TencentMap</t>
+          <t>GCJ02Street</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Карта Тенсент</t>
+          <t>улица GCJ02</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>droneList</t>
+          <t>TxMap</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Drone list</t>
+          <t>TencentMap</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Дроны</t>
+          <t>Карта Тенсент</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>color</t>
+          <t>droneList</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>color</t>
+          <t>Drone list</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Цвет</t>
+          <t>Дроны</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>model</t>
+          <t>color</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>color</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Модель</t>
+          <t>Цвет</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>azimuthDistance</t>
+          <t>model</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Azimuth distance</t>
+          <t>Model</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Расстояние по азимуту</t>
+          <t>Модель</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>deviceID</t>
+          <t>azimuthDistance</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Device ID</t>
+          <t>Azimuth distance</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>ID устройства</t>
+          <t>Расстояние по азимуту</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>updateTime</t>
+          <t>deviceID</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Update time</t>
+          <t>Device ID</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Время обновления</t>
+          <t>ID устройства</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>freq</t>
+          <t>updateTime</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Frequency</t>
+          <t>Update time</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>частота</t>
+          <t>Время обновления</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>band</t>
+          <t>freq</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Bandwidth</t>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Пропускная способность</t>
+          <t>частота</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>decode</t>
+          <t>band</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>decode</t>
+          <t>Bandwidth</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Расшифровать</t>
+          <t>Пропускная способность</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>detect</t>
+          <t>decode</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Detect</t>
+          <t>decode</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Обнаружение</t>
+          <t>Расшифровать</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>detect</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>online</t>
+          <t>Detect</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Онлайн</t>
+          <t>Обнаружение</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>offline</t>
+          <t>online</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Офлайн</t>
+          <t>Онлайн</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
         <is>
-          <t>detectList</t>
+          <t>offline</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Detect List</t>
+          <t>offline</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Дроны</t>
+          <t>Офлайн</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>locateDetect</t>
+          <t>detectList</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Locate/Detect</t>
+          <t>Detect List</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Найти/обнаружить</t>
+          <t>Дроны</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
         <is>
-          <t>resultList</t>
+          <t>locateDetect</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Detection Result</t>
+          <t>Locate/Detect</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Результаты</t>
+          <t>Найти/обнаружить</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>pilotMark</t>
+          <t>resultList</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>Detection Result</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Значок пилота</t>
+          <t>Результаты</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
         <is>
-          <t>displaySwitch</t>
+          <t>pilotMark</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Pilot</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Переключатель дисплея</t>
+          <t>Значок пилота</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
         <is>
-          <t>download</t>
+          <t>displaySwitch</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>download</t>
+          <t>Location</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Скачать</t>
+          <t>Переключатель дисплея</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>updatePlanError</t>
+          <t>download</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>update scenario error</t>
+          <t>download</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Не удалось обновить сценарий</t>
+          <t>Скачать</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>getPlanError</t>
+          <t>updatePlanError</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>get scenario error</t>
+          <t>update scenario error</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Не удалось получить сценарий</t>
+          <t>Не удалось обновить сценарий</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
+          <t>getPlanError</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>get scenario error</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Не удалось получить сценарий</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
           <t>edit</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
+      <c r="B75" t="inlineStr">
         <is>
           <t>edit</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>Редактировать</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" s="1" t="inlineStr"/>
+      <c r="C77" s="1" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>window:</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>savedSuccessfully</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Saved successfully</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Успешно сохранено</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>launch</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Launch</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Запустить</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>updateConfiguration</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Update Configuration</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Обновить конфигурацию</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>distance</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Distance</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Расстояние</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>detectOpen</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Detect-triggered power-on</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Включение по триггеру</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>autoOpen</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Auto Power-on</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Автоматическое включение</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>workMode</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Work mode</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Рабочий режим</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>drone</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Drone</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Дрон</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Модель</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>position &amp; distance</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>местоположение и дистанция</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>speed</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>speed</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Скорость</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Неизвестно</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>notLocated</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>not located</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Не находится</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>nonDifferentialPositioning</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>non-differential positioning</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Недифференциальное позиционирование</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>differentialPositioning</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>differential positioning</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Дифференциальное позиционирование</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>InvalidPPSTargeting</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Invalid PPS targeting</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Недопустимый таргетинг PPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>estimating</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>estimating</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Оценивание</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>deviceID</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>device id</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>ID устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Долгота</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Широта</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>latitudeAndLongitude</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>latitude and longitude</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Широта и Долгота</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>altitude</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>altitude</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Высота</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>satellites</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>satellites</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Количество спутников</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>positioningStatus</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>positioning status</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Статус позиционирования</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>hdop</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>HDOP</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Коэффициент точности горизонтального компонента</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>errorCode</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>errorCode</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Код ошибки</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>pilot</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>pilot</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Пилот</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>track</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Flight path</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Отслеживать</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>homePoint</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>home point</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Домашняя точка</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>pilotPosition</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>pilot position</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Позиция пилота</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>pilotCoordinates</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>pilot coordinates</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Координаты пилота</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>pilotLongitude</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>pilot longitude</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Долгота пилота</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>pilotLatitude</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>pilot latitude</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Широта пилота</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" s="1" t="inlineStr"/>
+      <c r="C114" s="1" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>msg:</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>ring_one</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>ring one</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Звонок один#</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>reset_ab</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>reset two relays</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Сбросить два реле</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>reset_a</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>reset a</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Сбросить a</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>reset_b</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>reset b</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Сбросить b</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>off_a</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>turn off a</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Выключить a</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>off_b</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>turn off b</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Выключить b</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>on_a</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>turn on a</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Включить a</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>on_b</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>turn on b</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Включить b</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>flush_hb</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>flush heartbeat</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>сбросить опрос</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>relayShowSetWarning</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Please be sure to set the hiding or display of the power amplifier according to the actual access situation.</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Обязательно настройте скрытие или отображение усилителя мощности</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>confirmEnterSpectrumTips</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Do you want to enter spectrum scanning?</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Вы хотите войти в сканирование спектра?</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>pleaseChooseEnterDevice</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Please choose the device you want to scan the frequency for</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите устройство, для которого вы хотите сканировать частоту</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>confirmTips</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Are you sure about the operation?</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Вы уверены в операции?</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>updateError</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Persistence configuration failed</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Не удалось обновить настройки</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>warningConfirm</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>This operation has certain risks, do you want to continue?</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Эта операция имеет определенные риски, вы хотите продолжить?</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>imgError</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Image parsing failed</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Ошибка синтаксического анализа изображения</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>noDroneName</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Please enter the name of the Drone</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите название дрона</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="inlineStr">
+        <is>
+          <t>rebootDevice</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>reboot device</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Перезагрузите устройство</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="inlineStr">
+        <is>
+          <t>defenseMode</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>defense mode</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Режим защиты</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="inlineStr">
+        <is>
+          <t>noFly</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>prohibited airspace</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Не летать</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="inlineStr">
+        <is>
+          <t>standby</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>standby</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>В ожидании</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="inlineStr">
+        <is>
+          <t>failedToGetDecoyDevice</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Failed to get GPS spoofing device</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Не удалось получить устройство-приманку</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="inlineStr">
+        <is>
+          <t>downloadMapConfirm2</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Please confirm that the map to be downloaded is correct and click download</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Подтвердите правильность загружаемой карты и нажмите «Загрузить».</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="inlineStr">
+        <is>
+          <t>downloadMapConfirm</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Whether or not to download the map of the selected area?</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Загружать ли карту выбранной области?</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>successfully</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Successful operation!</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Успешная операция!</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Operation failed!</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Операция не удалась!</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="inlineStr">
+        <is>
+          <t>mountDiskError</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Please select the disk to be mounted!</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите диск для монтирования!</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="inlineStr">
+        <is>
+          <t>userValidationError</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Authentication failed!</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Ошибка аутентификации!</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>noUserTips</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>No user defined, please try to set the password directly to create a user</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>В настоящее время пользователь не установлен, попробуйте установить пароль напрямую, чтобы создать пользователя</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="inlineStr">
+        <is>
+          <t>getDeviceInfoError</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Failed to get device information</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Не удалось получить данные об устройстве.</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="inlineStr">
+        <is>
+          <t>prompt</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Подсказка</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="inlineStr">
+        <is>
+          <t>restartDevicePrompt</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>This operation will reboot the device forever, do you want to continue?</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Эта операция перезагрузит устройство, хотите продолжить?</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>confirm</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Confirm</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Сохранить</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="inlineStr">
+        <is>
+          <t>cancel</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Cancel</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Отмена</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="inlineStr">
+        <is>
+          <t>restartSuccessfully</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>restart successfully</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Успешный перезапуск</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="inlineStr">
+        <is>
+          <t>restartFailed</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>restart failed</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>Перезагрузка не удалась</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="inlineStr">
+        <is>
+          <t>enterDroneNameTip</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Please type in Drone ID from White List</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите имя дрона из белого списка</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="inlineStr">
+        <is>
+          <t>enterDroneIDTip</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Please enter the drone ID</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите идентификатор дрона</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="inlineStr">
+        <is>
+          <t>noMoreData</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Data not available</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>Больше данных нет</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="inlineStr">
+        <is>
+          <t>changeLanguageTips</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Language switched successfully</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>Язык успешно переключен</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="inlineStr">
+        <is>
+          <t>longitudeCheckError</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Please enter correct longitude</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите правильную долготу</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="inlineStr">
+        <is>
+          <t>latitudeCheckError</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Please enter the correct latitude</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите правильную широту</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="inlineStr">
+        <is>
+          <t>longitudeLatitudeCheckError</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Please enter correct latitude and longitude</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите правильную широту и долготу</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="inlineStr">
+        <is>
+          <t>successfulOperationTips</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Successful operation</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>Успешная операция</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>failureOperationTips</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>operation failed</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>Операция не удалась</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="inlineStr">
+        <is>
+          <t>pleaseUploadFile</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Please upload the file</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Пожалуйста, загрузите файл</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>successfullySet</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>successfully set</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Успешно установлен</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="inlineStr">
+        <is>
+          <t>logoUploadFormatTips</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>The uploaded LOGO image can only be in PNG format!</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>Загруженное изображение ЛОГОТИПА может быть только в формате PNG!</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>logoUploadSizeTips</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>The size of the uploaded LOGO image cannot exceed 2MB!</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Размер загружаемого изображения ЛОГОТИПА не может превышать 2 МБ!</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="inlineStr">
+        <is>
+          <t>initialConfigurationPrompt</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>This operation will initialize configuration information, do you want to continue?</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Эта операция инициализирует информацию о конфигурации, следует ли продолжать?</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>copySuccessfully</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>copy successfully</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Скопировано успешно</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="inlineStr">
+        <is>
+          <t>zoomTips</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Please pay attention to the scaling rules, the maximum value cannot be smaller than the minimum value</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Пожалуйста, обратите внимание на правила масштабирования, максимальное значение не может быть меньше минимального значения.</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>longitudeTips</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Please pay attention to the size rule of longitude, the maximum value cannot be smaller than the minimum value</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Обратите внимание на долготу, максимальное значение не может быть меньше минимального значения</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="inlineStr">
+        <is>
+          <t>latitudeTips</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Please pay attention to the size rule of latitude, the maximum value cannot be smaller than the minimum value</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Обратите внимание на широту, максимальное значение не может быть меньше минимального значения.</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="inlineStr">
+        <is>
+          <t>layerError</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>The number of layers exceeds the limit, please reselect the appropriate latitude and longitude and zoom level</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Количество слоев превышает лимит, пожалуйста, повторно выберите соответствующую широту, долготу и уровень масштабирования</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="inlineStr">
+        <is>
+          <t>downloadCompleted</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Download completed</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>Загрузка завершена</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="inlineStr">
+        <is>
+          <t>stopDownloadTips</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Do you want to stop downloading? The downloaded progress will not be lost!</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>Вы хотите остановить загрузку? Скачанные части не будет потеряны!</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="inlineStr">
+        <is>
+          <t>cancelSuccess</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Cancel successfully</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>Успешно отменено</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="inlineStr">
+        <is>
+          <t>noPositionMsg</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>The selected flight path has not obtained the positioning result!</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>Выбранный трек не получил результат позиционирования!</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="inlineStr">
+        <is>
+          <t>noDetect</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>No detection results found!</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>Результаты обнаружения не найдены!</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="inlineStr">
+        <is>
+          <t>traceNoDetect</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>No positioning result for this flight path!</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Для этого трека нет результатов позиционирования!</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="inlineStr">
+        <is>
+          <t>drawCounterTips</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Please choose the way to set up countermeasure zone!</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите способ создания зоны противодействия!</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="inlineStr">
+        <is>
+          <t>drawDefenseTips</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Please choose the way to set up defense zone!</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите способ создания области предупреждения!</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="inlineStr">
+        <is>
+          <t>drawCounterLabel</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Please select the radius of the countermeasure zone (unit - meter)</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите радиус зоны противодействия (единица измерения - метр)</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="inlineStr">
+        <is>
+          <t>drawDefenseLabel</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Please select the radius of the defense area (unit - meter)</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите радиус зоны предупреждения (единица измерения - метр)</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="inlineStr">
+        <is>
+          <t>drawManually</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>draw manually</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>Нарисовать вручную</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="inlineStr">
+        <is>
+          <t>specifiedRadius</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>set radius</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>Указанный радиус</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="inlineStr">
+        <is>
+          <t>noUserSelect</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>No user defined, please choose to create a user or skip login authentication</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>В настоящее время пользователя нет. Выберите создать пользователя или пропустить проверку входа.</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="inlineStr">
+        <is>
+          <t>createUser</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Create user</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>Создать пользователя</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="inlineStr">
+        <is>
+          <t>skipVerification</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Skip authentication</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>Пропустить проверку</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="inlineStr">
+        <is>
+          <t>validateUsername</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Please enter user name</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>Введите имя пользователя</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>validatePassword</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Please enter user password</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>Введите пароль пользователя</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add all translation modules
</commit_message>
<xml_diff>
--- a/Шторм.xlsx
+++ b/Шторм.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C187"/>
+  <dimension ref="A1:C459"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2292,8 +2292,6 @@
           <t>msg:</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
@@ -3374,12 +3372,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Please select the radius of the countermeasure zone (unit - meter)</t>
+          <t>Please select the radius of the countermeasure zone (- meter)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Пожалуйста, выберите радиус зоны противодействия (единица измерения - метр)</t>
+          <t>Пожалуйста, выберите радиус зоны противодействия (единица - метр)</t>
         </is>
       </c>
     </row>
@@ -3391,12 +3389,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Please select the radius of the defense area (unit - meter)</t>
+          <t>Please select the radius of the defense area (- meter)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Пожалуйста, выберите радиус зоны предупреждения (единица измерения - метр)</t>
+          <t>Пожалуйста, выберите радиус зоны предупреждения (единица - метр)</t>
         </is>
       </c>
     </row>
@@ -3516,6 +3514,4432 @@
       <c r="C187" t="inlineStr">
         <is>
           <t>Введите пароль пользователя</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" s="1" t="inlineStr"/>
+      <c r="C189" s="1" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="inlineStr">
+        <is>
+          <t>set:</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="inlineStr">
+        <is>
+          <t>ssid</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>matching rule</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>SSID</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="inlineStr">
+        <is>
+          <t>setWifiConfigFailed</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Failed to set Wi-Fi configuration</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>Не удалось настроить конфигурацию Wi-Fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>getWifiConfigFailed</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Failed to get Wi-Fi configuration</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>Не удалось получить конфигурацию Wi-Fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="inlineStr">
+        <is>
+          <t>getWifiListFailed</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Failed to get Wi-Fi list</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>Не удалось получить список Wi-Fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="inlineStr">
+        <is>
+          <t>wifiManage</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Wi-Fi Management</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>Управление Wi-Fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="inlineStr">
+        <is>
+          <t>wifiList</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Wi-Fi List</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>Список Wi-Fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="inlineStr">
+        <is>
+          <t>deleteOrNot</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Delete or not?</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>Удалить или нет?</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="inlineStr">
+        <is>
+          <t>pleaseEnterCorrectRate</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Please enter the correct rate.</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите правильные данные</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="inlineStr">
+        <is>
+          <t>freqRateList</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Frequency rate list</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>Список блокировки частот</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="inlineStr">
+        <is>
+          <t>freqRangeTips</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Frequency input - 70M - 6000M</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>Диапазон ввода - 70M - 6000M</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="inlineStr">
+        <is>
+          <t>uploadExcelTips</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Uploaded files can only be in Excel format</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>Загружаемые файлы могут быть только в формате Excel</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="inlineStr">
+        <is>
+          <t>uploadExcelSizeTips</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Uploaded file size cannot exceed 2MB!</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>Размер загружаемого файла не может превышать 2MB!</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="inlineStr">
+        <is>
+          <t>uploadExcelConfirm</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>File parsed successfully, confirm to submit?</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>Файл успешно проанализирован, подтвердить отправку?</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="inlineStr">
+        <is>
+          <t>pleaseUploadCorrectExcel</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Please upload the correct format of excel file</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>Пожалуйста, загрузите файл Excel в правильном формате</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="inlineStr">
+        <is>
+          <t>aid</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Antenna ID</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>ID антенны</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="inlineStr">
+        <is>
+          <t>freqExists</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Frequency already exists</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>Частота уже существует</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="inlineStr">
+        <is>
+          <t>inputModeFailed</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Input model format is incorrect</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>Формат ввода модели неверен</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="inlineStr">
+        <is>
+          <t>inputFormatUnCorrect</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Input format is incorrect</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>Формат ввода неверен</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="inlineStr">
+        <is>
+          <t>configSuccess</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Configuration success</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>Конфигурация успешна</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="inlineStr">
+        <is>
+          <t>saveChange</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Save changes</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>Сохранить изменения</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="inlineStr">
+        <is>
+          <t>mode</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>Модель</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="inlineStr">
+        <is>
+          <t>pleaseSelectConfigId</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Please select the module to be configured</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите модуль для настройки</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="inlineStr">
+        <is>
+          <t>freqUnit</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Frequency (MHz)</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>Частота (МГц)</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="inlineStr">
+        <is>
+          <t>exports</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Export</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>Экспорт</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="inlineStr">
+        <is>
+          <t>RX2</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>(For side use)</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>(Для бокового использования)</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="inlineStr">
+        <is>
+          <t>getFreqListFailed</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Failed to get frequency information</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>Не удалось получить информацию о частоте</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="inlineStr">
+        <is>
+          <t>editFreq</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Edit frequency</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>Редактировать частоту</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="inlineStr">
+        <is>
+          <t>updatedConfig</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Configuration service</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>Сервис конфигурации</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="inlineStr">
+        <is>
+          <t>freq</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Frequency</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>Частота</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="inlineStr">
+        <is>
+          <t>freqModeMap</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Model frequency mapping table</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>Таблица сопоставления частот модели</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="inlineStr">
+        <is>
+          <t>freqList</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Frequency list</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>Список частот</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="inlineStr">
+        <is>
+          <t>mapPost</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Map File</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>Файл карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="inlineStr">
+        <is>
+          <t>traceList</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Trace List</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>Список маршрутов</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="inlineStr">
+        <is>
+          <t>decode</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Decode</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>Декодирование</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="inlineStr">
+        <is>
+          <t>detect</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Detect</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>Обнаружение</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>Статус</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="inlineStr">
+        <is>
+          <t>plan1</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Plan One</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>План 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="inlineStr">
+        <is>
+          <t>plan2</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Plan Two</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>План 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="inlineStr">
+        <is>
+          <t>plan3</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Plan Three</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>План 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="inlineStr">
+        <is>
+          <t>automaticAttackPlanTips</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Automatic attack plan will be synchronized to all devices that have opened automatic attack</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>Автоматический план атаки будет синхронизирован со всеми устройствами, которые открыли автоматическую атаку</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="inlineStr">
+        <is>
+          <t>autoCounterTime</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Strike duration</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>Продолжительность удара</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="inlineStr">
+        <is>
+          <t>autoCounterSwitch</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Automatic Attack Switch</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>Переключатель автоматической атаки</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="inlineStr">
+        <is>
+          <t>automaticAttackPlan</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Automatic Attack Plan</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>Автоматический план атаки</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="inlineStr">
+        <is>
+          <t>detectionThresholdTips</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>After detecting a certain number of times in a row, the attack is started</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>После обнаружения определенного количества раз подряд начинается атака</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="inlineStr">
+        <is>
+          <t>detectSet</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Detection Settings</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>Настройки обнаружения</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="inlineStr">
+        <is>
+          <t>useLockCoordinate</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Use Custom Coordinates</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>Задать координаты вручную</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="inlineStr">
+        <is>
+          <t>coordinate</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Coordinate</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>Координата</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="inlineStr">
+        <is>
+          <t>GNSSStatus</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>GNSS Status</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>Статус GNSS</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="inlineStr">
+        <is>
+          <t>latitudeAndLongitudeGps</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Latitude and Longitude Coordinates</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>Координаты широты и долготы</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="inlineStr">
+        <is>
+          <t>counterRelayControl</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Counter Relay Control</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>Управление реле</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="inlineStr">
+        <is>
+          <t>counterConfig</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Attack Configuration</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>Конфигурация атаки</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="inlineStr">
+        <is>
+          <t>manualConfig</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Manual</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>Ручная настройка</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>Нормальный</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="inlineStr">
+        <is>
+          <t>error</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>Ошибка</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="inlineStr">
+        <is>
+          <t>counterRecord</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Counter Record</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>Записи подавления</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="inlineStr">
+        <is>
+          <t>amplifierPosition</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Amplifier Position</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>Модуль подавителя</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="inlineStr">
+        <is>
+          <t>nameEdit</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Name Edit</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>Редактирование имени</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="inlineStr">
+        <is>
+          <t>dbUploadFormatTips</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Uploaded files can only be in DB format!</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>Загружаемые файлы могут быть только в формате DB!</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="inlineStr">
+        <is>
+          <t>submit</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Submit</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>Отправить</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="inlineStr">
+        <is>
+          <t>traceClearTimeout</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Trace Data Timeout Clear</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>Очистка данных маршрутов по таймауту</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="inlineStr">
+        <is>
+          <t>selectFile</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Select File</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>Выберите файл</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="inlineStr">
+        <is>
+          <t>mapImport</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Map Import</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>Импорт карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="inlineStr">
+        <is>
+          <t>mapDelete</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Map Delete</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>Удалить карту</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="inlineStr">
+        <is>
+          <t>mapManage</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Map Manage</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>Управление картой</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="inlineStr">
+        <is>
+          <t>featureMenu</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Menu</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>Настройки</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="inlineStr">
+        <is>
+          <t>moduleConfig</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Setting</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>Конф. модуля</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="inlineStr">
+        <is>
+          <t>relayConfig</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Relay</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>Конф. реле</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="inlineStr">
+        <is>
+          <t>modeListTips</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>- You can search or manage the list of model references here.</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>- Здесь вы можете искать или управлять списком ссылок на модели</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="inlineStr">
+        <is>
+          <t>modeList</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Model list</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>Список моделей</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="inlineStr">
+        <is>
+          <t>modeName</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>Название модели</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="inlineStr">
+        <is>
+          <t>modeIdRepeat</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Model ID already exists!</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>Идентификатор модели уже существует!</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="inlineStr">
+        <is>
+          <t>specialModelDetectionSwitch</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Special model detection switch</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>Переключатель обнаружения специальной модели</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="inlineStr">
+        <is>
+          <t>specialModelDetectionSwitchTips</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Whether to display the detection results of special models</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Отображать ли результаты обнаружения специальных моделей</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="inlineStr">
+        <is>
+          <t>deleteMapDB</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Delete map files and restart the service</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Удалите файлы карты и перезапустите службу</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="inlineStr">
+        <is>
+          <t>manualCounterWarning</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Manual counter is unavailable in automatic attack mode</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Невозможно вручную контратаковать в режиме автоматической атаки</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="inlineStr">
+        <is>
+          <t>relayDev</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>relay</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Реле</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="inlineStr">
+        <is>
+          <t>manualCounter</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>manual countermeasure</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Ручное противодействие</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="inlineStr">
+        <is>
+          <t>detectionThreshold</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>detection threshold</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Порог обнаружения</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="inlineStr">
+        <is>
+          <t>relay</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Relay status</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Состояние реле</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="inlineStr">
+        <is>
+          <t>automatic</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Unattended</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Авт. атака</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="inlineStr">
+        <is>
+          <t>interferenceTime</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Interference time</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Время помех</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="inlineStr">
+        <is>
+          <t>module</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Тип модуля</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="inlineStr">
+        <is>
+          <t>devSet</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Devices</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="inlineStr">
+        <is>
+          <t>moduleSet</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Module management</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Управление модулями</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="inlineStr">
+        <is>
+          <t>autoSetTime</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>set time automatically</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Установить время автоматически</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="inlineStr">
+        <is>
+          <t>selectDateTime</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Select date time</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>выберите дату и время</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="inlineStr">
+        <is>
+          <t>timezoneSet</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>time zone</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Часовой пояс</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="inlineStr">
+        <is>
+          <t>serverTime</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Server time</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Серверное время</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="inlineStr">
+        <is>
+          <t>timeSet</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Time Setting</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Настройки времени</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="inlineStr">
+        <is>
+          <t>trojanDevice</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>GPS spoofing device</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Обманное устройство</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="inlineStr">
+        <is>
+          <t>fileDownload</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Download File</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Скачать документ</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="inlineStr">
+        <is>
+          <t>downloadMapTips</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>You can also use the download map tool in the toolbox to specify an area to download</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Вы можете скачать часть карты, используя модуль скачивания карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="inlineStr">
+        <is>
+          <t>deleteLog</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Delete the log file directory</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Удалить каталог файла журнала</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="inlineStr">
+        <is>
+          <t>diskUsage</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>View disk usage</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Просмотр использования диска</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="inlineStr">
+        <is>
+          <t>deleteCache</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Clear cache</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Очистить кэш</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Протестировать</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="inlineStr">
+        <is>
+          <t>networkTest</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>network test</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Сетевой тест</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="inlineStr">
+        <is>
+          <t>executeScript</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Execute script</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Выполнить скрипт</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="inlineStr">
+        <is>
+          <t>ipDetails</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Query IP details</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Запрос IP-деталей</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="inlineStr">
+        <is>
+          <t>ScriptTool</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Script Tool</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Инструмент изменения скрипта</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="inlineStr">
+        <is>
+          <t>wifiConnect</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>WiFi Connect</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Wi-Fi соединение</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="inlineStr">
+        <is>
+          <t>detectDisplayTips</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Whether to display the detection results(Turning off the display will mask the detection alarm)</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Отображать ли результаты обнаружения (отключение дисплея скроет тревогу обнаружения)</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="inlineStr">
+        <is>
+          <t>detectDisplay</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Detect display Settings</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Настройки отображения датчика</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="inlineStr">
+        <is>
+          <t>patchMap</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Update map file</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Обновить файл карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="inlineStr">
+        <is>
+          <t>patchServer</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Update the server program</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Обновите серверную программу</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="inlineStr">
+        <is>
+          <t>connect</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>connect</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Соединить</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="inlineStr">
+        <is>
+          <t>mount</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>mount</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Установить</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="inlineStr">
+        <is>
+          <t>WifSsidTips</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>please enter SSID</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите ssid</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="inlineStr">
+        <is>
+          <t>WifPskTips</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Please enter PSK</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите PSK</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="inlineStr">
+        <is>
+          <t>diskSelectTips</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Please select the disk to be mounted</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите диск для монтирования</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="inlineStr">
+        <is>
+          <t>diskWifTips</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Please select the network interface card to be connected</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите сетевую карту для подключения</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="inlineStr">
+        <is>
+          <t>files</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>File System</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Файловая система</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="inlineStr">
+        <is>
+          <t>devIp</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Device IP</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>IP-адрес устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="inlineStr">
+        <is>
+          <t>serverVersion</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Server version No</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Версия сервера</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="inlineStr">
+        <is>
+          <t>otherInfo</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Other Information</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Другая информация</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="inlineStr">
+        <is>
+          <t>reset</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>reset</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Сброс настроек</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="inlineStr">
+        <is>
+          <t>resetUserPrompt</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>If the password or username is left blank, the current user will be logged out</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Если пароль или имя пользователя оставить пустыми, текущий пользователь выйдет из системы</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="inlineStr">
+        <is>
+          <t>resetUser</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>reset user</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Сбросить пользователя</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>нет</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>да</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="inlineStr">
+        <is>
+          <t>skipVerification</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Whether to enable login verification</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Включить ли проверку входа</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="inlineStr">
+        <is>
+          <t>skip</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>skip</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Пропустить</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="inlineStr">
+        <is>
+          <t>verification</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>authentication</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Проверка</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="inlineStr">
+        <is>
+          <t>loginVerification</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Login verification</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Проверка входа</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="inlineStr">
+        <is>
+          <t>SecuritySet</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Security Settings</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>Настройки безопасности</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="inlineStr">
+        <is>
+          <t>displaySet</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Display Setting</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Настройка экрана</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="inlineStr">
+        <is>
+          <t>platformDisplaySettings</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>UI display settings</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Настройки отображения платформы</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="inlineStr">
+        <is>
+          <t>platformTitleSettings</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>UI Title settings</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Настройки названия платформы</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="inlineStr">
+        <is>
+          <t>titleSettingTips</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Please enter the UI title to be modified, by default if blank</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Пожалуйста, введите название платформы, которую нужно изменить, по умолчанию это поле пусто</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="inlineStr">
+        <is>
+          <t>showLogo</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Whether to display the logo</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Отображать ли логотип</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Показать</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="inlineStr">
+        <is>
+          <t>hide</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>hide</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Спрятать</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="inlineStr">
+        <is>
+          <t>deviceDisplaySettings</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Device display settings</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Настройки дисплея устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="inlineStr">
+        <is>
+          <t>customLatitudeAndLongitude</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>custom latitude and longitude</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Пользовательская широта и долгота</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Сохранить</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="inlineStr">
+        <is>
+          <t>isLock</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Whether to fix</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Блокирован?</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="inlineStr">
+        <is>
+          <t>locked</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Заблокирован</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="inlineStr">
+        <is>
+          <t>unlock</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Not fixed</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Разблокирован</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="inlineStr">
+        <is>
+          <t>deviceAnimationEffectSettings</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Device animation effect settings</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Настройки эффекта анимации устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="inlineStr">
+        <is>
+          <t>dynamicWarningRangeSettingTips</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>The dynamic alarming range is based on the effective radius of the defense range</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Динамический диапазон предупреждения основан на эффективном радиусе зоны защиты.</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="inlineStr">
+        <is>
+          <t>meters</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Meter</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>метр</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="inlineStr">
+        <is>
+          <t>trackDisplay</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Flight path display</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Отобразить трек</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="inlineStr">
+        <is>
+          <t>trackNumberLimit</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Flight path limit</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>Ограничение количества треков</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="inlineStr">
+        <is>
+          <t>pleaseChoose</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>please choose</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="inlineStr">
+        <is>
+          <t>tipsForSettingTheNumberOfTracks</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Limiting flight paths will reduce false alarms displayed</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Ограничение количества трасс снижает количество отображаемых ложных тревог.</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="inlineStr">
+        <is>
+          <t>timeoutTraceCleanup</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Expired flight path purge</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Очистка трассировки тайм-аута</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="inlineStr">
+        <is>
+          <t>timeoutCleanupEnabled</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Expired flight path purging enabled</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>Очистка по тайм-ауту включена</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="inlineStr">
+        <is>
+          <t>timeoutCleanupUnEnabled</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Expired flight path purging not enabled</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Очистка по тайм-ауту выключена</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="inlineStr">
+        <is>
+          <t>trackTimeoutSettingPrompt</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>If the update request is not accepted within set time, the expired flight path on the interface will be purged</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>Если обновление трека не будет подтверждено после установленного времени, трек на интерфейсе будет очищен</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="inlineStr">
+        <is>
+          <t>isShowDefense</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Whether to display the defense area on the home page</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Отображать ли область предупреждения на главной странице</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="inlineStr">
+        <is>
+          <t>isShowCounter</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Whether to display the countermeasure area on the home page</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>Отображать зону противодействия на главной странице</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="inlineStr">
+        <is>
+          <t>clearConfigurationCache</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Clear configuration cache</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Очистить кеш конфигурации</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>clear</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Очистить</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="inlineStr">
+        <is>
+          <t>clearPrompt</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Clear cached configuration and reset to initial values</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Очистить кешированную конфигурацию и сбросить до начальных значений</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="inlineStr">
+        <is>
+          <t>alarmSettings</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Alarm Settings</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>Настройки сигнала</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="inlineStr">
+        <is>
+          <t>platformAlarmSwitch</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Alarm switch</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Переключатель сигнализации платформы</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="inlineStr">
+        <is>
+          <t>voiceAlarm</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>sound alarm</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Звуковая сигнализация</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="inlineStr">
+        <is>
+          <t>whetherToUseSoundAlarm</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Whether to use sound alarm</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>Использовать ли звуковой сигнал</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="inlineStr">
+        <is>
+          <t>lightWarning</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>flashing alarm</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>Мигающее предупреждение</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="inlineStr">
+        <is>
+          <t>whetherToSseFlashingWarning</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Whether to use flashing alarm</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>Использовать ли мигающее предупреждение</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="inlineStr">
+        <is>
+          <t>platformLOGOSetting</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Logo settings</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Настройка ЛОГОТИПА платформы</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="inlineStr">
+        <is>
+          <t>uploadTips</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Please upload logo file in PNG format</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Пожалуйста, загрузите ЛОГОТИП платформы для изменения в формате PNG</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="inlineStr">
+        <is>
+          <t>mapDownload</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Map Download</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>Загрузка карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="inlineStr">
+        <is>
+          <t>mapDownloadTips</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>During the map download, if there is no update progress for a long time, you may try to cancel and re-download, the downloaded progress will not be lost</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Если долго нет прогресса обновления карты, можно попробовать отменить и заново скачать, загруженный прогресс не потеряется</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="inlineStr">
+        <is>
+          <t>cancelDownload</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>cancel download</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>Отменить загрузку</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="inlineStr">
+        <is>
+          <t>mapProvider</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>map provider</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>Поставщик карт</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="inlineStr">
+        <is>
+          <t>mapProviderID</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Please select a map provider ID</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>Выберите идентификатор поставщика карт</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="inlineStr">
+        <is>
+          <t>minZoom</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>minimum zoom</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>Минимальный зум</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="inlineStr">
+        <is>
+          <t>maxZoom</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>maximum zoom</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>Максимальный зум</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="inlineStr">
+        <is>
+          <t>minZoomTips</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Minimum zoom recommended &gt;4</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>Рекомендуемый минимальный зум &gt;4</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="inlineStr">
+        <is>
+          <t>maxZoomTips</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>For maximum zoom, 18 is recommended, most maps have no images when &gt; 18</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>Максимальный масштаб, рекомендуется 18, большинство карт &gt; 18 не имеют изображений</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="inlineStr">
+        <is>
+          <t>maxLat</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>latitude maximum</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>Максимальная широта</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="inlineStr">
+        <is>
+          <t>minLat</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>latitude minimum</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>Минимальная широта</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="inlineStr">
+        <is>
+          <t>minLng</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>longitude minimum</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>Минимальная долгота</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="inlineStr">
+        <is>
+          <t>maxLng</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>longitude max</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>Максимальная долгота</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="inlineStr">
+        <is>
+          <t>downloadNow</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>download now</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>Скачать</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="inlineStr">
+        <is>
+          <t>pleaseSelectLayer</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Please select a layer to download</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите слой для загрузки</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="inlineStr">
+        <is>
+          <t>detectWarning</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Detection alarm</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>Сигнализация обнаружения</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="inlineStr">
+        <is>
+          <t>detectWarningTips</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Immediately alarm if there is a detection result</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>Предупреждение о результате обнаружения</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="inlineStr">
+        <is>
+          <t>second</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>second</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>Второй</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="inlineStr">
+        <is>
+          <t>deviceLockTips</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Unfix to get device GPS information</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>Разблокируйте, чтобы получить информацию GPS устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="inlineStr">
+        <is>
+          <t>dataClearing</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Data purge</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>Очистка данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="inlineStr">
+        <is>
+          <t>clearDatabase</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Purge database</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>Очистить базу данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="inlineStr">
+        <is>
+          <t>clearDatabaseTips</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>This operation will delete all data in the detection and flight path lists, please use with caution!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>Эта операция удалит все данные в списке обнаружения и отслеживания, пожалуйста, используйте с осторожностью!</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="inlineStr">
+        <is>
+          <t>initialDatabasePrompt</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>This operation will purge all data in the database, do you want to continue?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>Эта операция очистит все данные в базе данных, следует ли продолжить?</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="inlineStr">
+        <is>
+          <t>altitudeCalibrationAltitude</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Altitude Value Calibration</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>Калибровка высоты над уровнем моря</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="inlineStr">
+        <is>
+          <t>planSet</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Scenario display settings</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>Настройки отображения сценария</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="inlineStr">
+        <is>
+          <t>drawCounter</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Set countermeasure zone</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>Зона противодействия</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="inlineStr">
+        <is>
+          <t>drawDefense</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Set defence zone</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>Зона предупреждения</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="inlineStr">
+        <is>
+          <t>alarmVolume</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Alarm volume</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>Громкость будильника</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="inlineStr">
+        <is>
+          <t>customMap</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Custom map source</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>Пользовательский источник карты</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="B383" s="1" t="inlineStr"/>
+      <c r="C383" s="1" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="inlineStr">
+        <is>
+          <t>record:</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1" t="inlineStr">
+        <is>
+          <t>startRelay</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Action Module</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>Модуль действия</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="inlineStr">
+        <is>
+          <t>recordList</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>History</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>Записи</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1" t="inlineStr">
+        <is>
+          <t>detectList</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Detection record</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>Записи обнаружения</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1" t="inlineStr">
+        <is>
+          <t>timeSelect</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Time selection</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>Период</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>до</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1" t="inlineStr">
+        <is>
+          <t>startTime</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Starting time</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>Время начала</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="inlineStr">
+        <is>
+          <t>endTime</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>End Time</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>Время окончания</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1" t="inlineStr">
+        <is>
+          <t>search</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>search</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>Поиск</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>Время</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="inlineStr">
+        <is>
+          <t>device</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>device</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Оборудование</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Частота</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="1" t="inlineStr">
+        <is>
+          <t>nameAndSsid</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Drone name/ SSID</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>Имя дрона/ssid</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="inlineStr">
+        <is>
+          <t>moduleAndMac</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>model/mac</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Модель дрона/mac</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="1" t="inlineStr">
+        <is>
+          <t>isWhite</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Whether to whitelist</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Вносить ли в белый список</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>serial No</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Серийный номер</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="B401" s="1" t="inlineStr"/>
+      <c r="C401" s="1" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="inlineStr">
+        <is>
+          <t>playback:</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="1" t="inlineStr">
+        <is>
+          <t>playback</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Data Playback</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Воспроизведение</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="1" t="inlineStr">
+        <is>
+          <t>checkTrace</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>select file to play</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>Выбрать файл воспроизведения</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="1" t="inlineStr">
+        <is>
+          <t>traceId</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Flight path ID</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>Идентификатор трека</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="1" t="inlineStr">
+        <is>
+          <t>search</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>search</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Поиск</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="1" t="inlineStr">
+        <is>
+          <t>checked</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>selected</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>Выбран</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="1" t="inlineStr">
+        <is>
+          <t>play</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>play</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>проиграть</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="1" t="inlineStr">
+        <is>
+          <t>selectPlaybackSpeed</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Please select playback speed</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>Выберите скорость воспроизведения</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="1" t="inlineStr">
+        <is>
+          <t>traceList</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Flight path list</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>Треки</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="1" t="inlineStr">
+        <is>
+          <t>selectTraceTips</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Please tick the flight path to be played back</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>Пожалуйста, отметьте трек, который нужно воспроизвести</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="B413" s="1" t="inlineStr"/>
+      <c r="C413" s="1" t="inlineStr"/>
+    </row>
+    <row r="414">
+      <c r="A414" s="1" t="inlineStr">
+        <is>
+          <t>analyze:</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="1" t="inlineStr">
+        <is>
+          <t>timeSelect</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Time selection</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>Выбор времени</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Drone control data visualization</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>Визуализация данных управления БЛА</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="1" t="inlineStr">
+        <is>
+          <t>checkAll</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>selectAll</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>Выбрать все</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>Продолжительность</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="1" t="inlineStr">
+        <is>
+          <t>discoveryTime</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Discovered time</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>Найдите время</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="1" t="inlineStr">
+        <is>
+          <t>pageExport</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Export</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>Экспорт страницы</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="1" t="inlineStr">
+        <is>
+          <t>startCluster</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Heat map of flight path starting point</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>Тепловая карта точки начала траектории</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="1" t="inlineStr">
+        <is>
+          <t>pilotCluster</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Heat map of pilot position</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>Тепловая карта положения пилота</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="1" t="inlineStr">
+        <is>
+          <t>quantityDistributionCurve</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Number distribution curve</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>Кривая распределения количества</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="1" t="inlineStr">
+        <is>
+          <t>detectNumber</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Number of detections</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>Количество обнаружений</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="1" t="inlineStr">
+        <is>
+          <t>traceNumber</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Flight path points</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>Точки трека</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="1" t="inlineStr">
+        <is>
+          <t>invasionSorties</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Intrusion sorties</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>Вылеты вторжения</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="1" t="inlineStr">
+        <is>
+          <t>sorties</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>sorties</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>Вылеты</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="1" t="inlineStr">
+        <is>
+          <t>invasionDuration</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Total intrusion time (minutes)</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>Общее время вторжения (минуты)</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="1" t="inlineStr">
+        <is>
+          <t>eventTrend</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Event trend</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>Тренд событий</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="1" t="inlineStr">
+        <is>
+          <t>timeDistribution</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Time Distribution</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>Распределение времени</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="1" t="inlineStr">
+        <is>
+          <t>pleaseSelectTheNumberOfIntervals</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Please select the number of intervals</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите количество интервалов</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="1" t="inlineStr">
+        <is>
+          <t>timeInterval4</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>4 time nodes</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>Количество узлов времени 4</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="1" t="inlineStr">
+        <is>
+          <t>timeInterval6</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>6 time nodes</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>Количество узлов времени 6</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="1" t="inlineStr">
+        <is>
+          <t>timeInterval8</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>8 time nodes</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>Количество узлов времени 8</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="1" t="inlineStr">
+        <is>
+          <t>timeInterval9</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>9 time nodes</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>Количество узлов времени 9</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="1" t="inlineStr">
+        <is>
+          <t>timeInterval11</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>11 time nodes</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>Количество узлов времени 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="1" t="inlineStr">
+        <is>
+          <t>lastWeek</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Previous week</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>Прошлая неделя</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="1" t="inlineStr">
+        <is>
+          <t>lastMonth</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Previous month</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>Прошлый месяц</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="1" t="inlineStr">
+        <is>
+          <t>lastThreeMonths</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Previous three months</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>Последние три месяца</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="1" t="inlineStr">
+        <is>
+          <t>totalDiscovery</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>total discovery</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>За всё время</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="1" t="inlineStr">
+        <is>
+          <t>modelProportion</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Model proportion</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>Пропорции модели</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="1" t="inlineStr">
+        <is>
+          <t>goback</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>home page</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>Вернуться на главную</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="B444" s="1" t="inlineStr"/>
+      <c r="C444" s="1" t="inlineStr"/>
+    </row>
+    <row r="445">
+      <c r="A445" s="1" t="inlineStr">
+        <is>
+          <t>spectrum:</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr"/>
+      <c r="C445" t="inlineStr"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="1" t="inlineStr">
+        <is>
+          <t>spectrumInit</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Device initializing</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>Инициализация устройства</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="1" t="inlineStr">
+        <is>
+          <t>spectrumRange</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Scan range</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>Диапазон развертки</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="1" t="inlineStr">
+        <is>
+          <t>spectrum</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Spectrum</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>Спектр</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="1" t="inlineStr">
+        <is>
+          <t>spectrumMonitoring</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Spectrum Monitoring</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>Мониторинг Спектра</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="1" t="inlineStr">
+        <is>
+          <t>configSettings</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Configuration Settings</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>Настройка параметров</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="1" t="inlineStr">
+        <is>
+          <t>frequencySelect</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Frequency Selection</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>Выбор частоты</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="inlineStr">
+        <is>
+          <t>rbwSelect</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Please select RBW</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>Пожалуйста, выберите RBW</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="1" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>Открыть</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="1" t="inlineStr">
+        <is>
+          <t>sensor</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Sensor</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>Датчик</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="1" t="inlineStr">
+        <is>
+          <t>playback</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Playback</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>Воспроизведение</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="1" t="inlineStr">
+        <is>
+          <t>pause</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Pause</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>Пауза</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="1" t="inlineStr">
+        <is>
+          <t>strength</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Strength</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>Сила</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="1" t="inlineStr">
+        <is>
+          <t>spectrumStop</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Spectrum Scanning Stopped</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>Сканирование спектра остановлено</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="1" t="inlineStr">
+        <is>
+          <t>spectrumStart</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Spectrum Scanning Started</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>Сканирование спектра начато</t>
         </is>
       </c>
     </row>

</xml_diff>